<commit_message>
modified mental health projeact dashboard
</commit_message>
<xml_diff>
--- a/Excel Projects/Mental Health Disorders project.xlsx
+++ b/Excel Projects/Mental Health Disorders project.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\White\Desktop\Portfolio Projects\Excel Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D6CC17-2375-48EA-A17E-E434B8EC64B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C0AB42-B2BA-41EA-BA84-7E11BDD7385C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="3" xr2:uid="{8E5352D9-4E44-44C7-B94E-43753D1FA9DE}"/>
   </bookViews>
@@ -1449,7 +1449,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="103">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -1625,28 +1625,127 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="173" formatCode="0.0"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="173" formatCode="0.0"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.000"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.000"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="0.0000"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="0.0000"/>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1710,12 +1809,12 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Slicer Style 1" pivot="0" table="0" count="8" xr9:uid="{89A6B7F8-D798-41EE-9776-3CB870E600C2}">
-      <tableStyleElement type="wholeTable" dxfId="69"/>
-      <tableStyleElement type="headerRow" dxfId="68"/>
+      <tableStyleElement type="wholeTable" dxfId="102"/>
+      <tableStyleElement type="headerRow" dxfId="101"/>
     </tableStyle>
     <tableStyle name="SlicerStyleDark5 2" pivot="0" table="0" count="10" xr9:uid="{B767567C-B5C0-42C2-B7C7-B6F49C7EBF8E}">
-      <tableStyleElement type="wholeTable" dxfId="67"/>
-      <tableStyleElement type="headerRow" dxfId="66"/>
+      <tableStyleElement type="wholeTable" dxfId="100"/>
+      <tableStyleElement type="headerRow" dxfId="99"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3364,25 +3463,25 @@
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>8</c:v>
@@ -3397,25 +3496,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>4</c:v>
@@ -11037,7 +11136,7 @@
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 5556"/>
+            <a:gd name="adj" fmla="val 3217"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -11112,7 +11211,7 @@
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 5556"/>
+            <a:gd name="adj" fmla="val 2047"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -11187,7 +11286,7 @@
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 5556"/>
+            <a:gd name="adj" fmla="val 3244"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -11262,7 +11361,7 @@
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 6141"/>
+            <a:gd name="adj" fmla="val 2118"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -11337,7 +11436,7 @@
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 5556"/>
+            <a:gd name="adj" fmla="val 2632"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -11412,7 +11511,7 @@
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 5556"/>
+            <a:gd name="adj" fmla="val 2632"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -11562,7 +11661,7 @@
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 5556"/>
+            <a:gd name="adj" fmla="val 2632"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -11637,7 +11736,7 @@
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 5556"/>
+            <a:gd name="adj" fmla="val 3217"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -16820,7 +16919,7 @@
     <dataField name="Average of Concentration" fld="16" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="48">
+    <format dxfId="96">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -16932,7 +17031,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{33438ED4-C5CE-45A7-93CD-A52DCDC8FA3E}" name="Exhaustion level" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{33438ED4-C5CE-45A7-93CD-A52DCDC8FA3E}" name="Exhaustion level" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="F28:G32" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="19">
     <pivotField dataField="1" showAll="0"/>
@@ -17019,8 +17118,26 @@
   <dataFields count="1">
     <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="3">
     <chartFormat chart="4" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="4" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -17417,7 +17534,7 @@
     <dataField name="Average of Optimisim" fld="17" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="54">
+    <format dxfId="98">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -17500,7 +17617,7 @@
     <dataField name="Average of Sexual Activity" fld="15" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="52">
+    <format dxfId="97">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -17517,7 +17634,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5B60E55B-B705-4BE3-A2E0-C51618093F88}" name="Expert Diagnosis" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5B60E55B-B705-4BE3-A2E0-C51618093F88}" name="Expert Diagnosis" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="20">
   <location ref="B7:C11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="19">
     <pivotField dataField="1" showAll="0"/>
@@ -17698,7 +17815,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7A059DB6-E0C4-49B2-9545-AFB5043E0D09}" name="Sleep Disorder levels" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7A059DB6-E0C4-49B2-9545-AFB5043E0D09}" name="Sleep Disorder levels" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
   <location ref="J28:K32" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="19">
     <pivotField dataField="1" showAll="0"/>
@@ -18095,15 +18212,15 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
       <items count="9">
+        <item x="6"/>
+        <item x="1"/>
         <item x="0"/>
-        <item x="1"/>
+        <item x="3"/>
         <item x="2"/>
-        <item x="3"/>
+        <item x="5"/>
         <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
         <item x="7"/>
         <item t="default"/>
       </items>
@@ -25778,7 +25895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3350A5-98BE-47FD-8168-25FC3B516B83}">
   <dimension ref="A1:S121"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
@@ -32957,7 +33074,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
@@ -33154,10 +33271,10 @@
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" s="5">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -33170,10 +33287,10 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C19" s="5">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -33198,10 +33315,10 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C21" s="5">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>34</v>
@@ -33238,10 +33355,10 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C23" s="5">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
modified mental health project
</commit_message>
<xml_diff>
--- a/Excel Projects/Mental Health Disorders project.xlsx
+++ b/Excel Projects/Mental Health Disorders project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\White\Desktop\Portfolio Projects\Excel Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C0AB42-B2BA-41EA-BA84-7E11BDD7385C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E356AD-4501-485F-8938-9F4016B76E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="3" xr2:uid="{8E5352D9-4E44-44C7-B94E-43753D1FA9DE}"/>
   </bookViews>
@@ -28,7 +28,7 @@
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="56" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4291" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4277" uniqueCount="285">
   <si>
     <t>Patient Number</t>
   </si>
@@ -1402,8 +1402,8 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1449,178 +1449,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="103">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
+  <dxfs count="46">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -1809,12 +1638,12 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Slicer Style 1" pivot="0" table="0" count="8" xr9:uid="{89A6B7F8-D798-41EE-9776-3CB870E600C2}">
-      <tableStyleElement type="wholeTable" dxfId="102"/>
-      <tableStyleElement type="headerRow" dxfId="101"/>
+      <tableStyleElement type="wholeTable" dxfId="45"/>
+      <tableStyleElement type="headerRow" dxfId="44"/>
     </tableStyle>
     <tableStyle name="SlicerStyleDark5 2" pivot="0" table="0" count="10" xr9:uid="{B767567C-B5C0-42C2-B7C7-B6F49C7EBF8E}">
-      <tableStyleElement type="wholeTable" dxfId="100"/>
-      <tableStyleElement type="headerRow" dxfId="99"/>
+      <tableStyleElement type="wholeTable" dxfId="43"/>
+      <tableStyleElement type="headerRow" dxfId="42"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2434,19 +2263,10 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Chart'!$B$8:$B$11</c:f>
+              <c:f>'Pivot Chart'!$B$8</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Bipolar Type-1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Bipolar Type-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Depression</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>Normal</c:v>
                 </c:pt>
               </c:strCache>
@@ -2454,28 +2274,19 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Chart'!$C$8:$C$11</c:f>
+              <c:f>'Pivot Chart'!$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1B1F-4F35-AD04-CFB9A8FDF060}"/>
+              <c16:uniqueId val="{00000000-7137-4143-9FA7-B267A09FBEDE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2898,70 +2709,22 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Chart'!$F$8:$F$16</c:f>
+              <c:f>'Pivot Chart'!$F$8</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Chart'!$G$8:$G$16</c:f>
+              <c:f>'Pivot Chart'!$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -2969,7 +2732,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3B75-4649-92C0-BF9A27A92878}"/>
+              <c16:uniqueId val="{00000000-37A5-408C-8B91-C678CF0356E1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3459,72 +3222,36 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Chart'!$B$17:$B$24</c:f>
+              <c:f>'Pivot Chart'!$B$17:$B$18</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Chart'!$C$17:$C$24</c:f>
+              <c:f>'Pivot Chart'!$C$17:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-24F0-4C77-AC76-C212B05437A4}"/>
+              <c16:uniqueId val="{00000000-3D60-4551-8D93-9E37CE533C92}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4013,70 +3740,22 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Chart'!$J$8:$J$16</c:f>
+              <c:f>'Pivot Chart'!$J$8</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Chart'!$K$8:$K$16</c:f>
+              <c:f>'Pivot Chart'!$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -4084,7 +3763,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-432F-4345-B598-363065F18C30}"/>
+              <c16:uniqueId val="{00000000-FBE0-4C44-A32E-67A4E41DF358}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4561,48 +4240,30 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Chart'!$F$21:$F$24</c:f>
+              <c:f>'Pivot Chart'!$F$21</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Most-Often</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Seldom</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>Sometimes</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Usually</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Chart'!$G$21:$G$24</c:f>
+              <c:f>'Pivot Chart'!$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E950-4A2E-92C1-A8F45A9EEA5A}"/>
+              <c16:uniqueId val="{00000000-AF52-4F3C-B8A5-79C431F491D1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5015,48 +4676,30 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Chart'!$F$29:$F$32</c:f>
+              <c:f>'Pivot Chart'!$F$29</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Most-Often</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Seldom</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>Sometimes</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Usually</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Chart'!$G$29:$G$32</c:f>
+              <c:f>'Pivot Chart'!$G$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7B31-4A3C-A345-658DE912137A}"/>
+              <c16:uniqueId val="{00000000-8680-4DF4-8EBB-526DE234739F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5469,19 +5112,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Chart'!$J$29:$J$32</c:f>
+              <c:f>'Pivot Chart'!$J$29:$J$30</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Most-Often</c:v>
+                  <c:v>Seldom</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Seldom</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sometimes</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>Usually</c:v>
                 </c:pt>
               </c:strCache>
@@ -5489,28 +5126,22 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Chart'!$K$29:$K$32</c:f>
+              <c:f>'Pivot Chart'!$K$29:$K$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-963C-42F4-85F5-BA04686CE37D}"/>
+              <c16:uniqueId val="{00000000-AE58-43D5-9C2F-BE9098368803}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5982,110 +5613,33 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-7172-4253-8422-F1B0D5CD265E}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-7172-4253-8422-F1B0D5CD265E}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-7172-4253-8422-F1B0D5CD265E}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-7172-4253-8422-F1B0D5CD265E}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Chart'!$J$21:$J$24</c:f>
+              <c:f>'Pivot Chart'!$J$21</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Most-Often</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Seldom</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>Sometimes</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Usually</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Chart'!$K$21:$K$24</c:f>
+              <c:f>'Pivot Chart'!$K$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-7172-4253-8422-F1B0D5CD265E}"/>
+              <c16:uniqueId val="{00000008-AEAB-4263-BDB9-D9A992FE0312}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12934,8 +12488,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="50" name="Mood Swing">
@@ -12958,7 +12512,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -13012,8 +12566,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="52" name="Overthinking">
@@ -13036,7 +12590,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -13090,8 +12644,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="54" name="Admit Mistakes">
@@ -13114,7 +12668,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -13530,7 +13084,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:t>120</a:t>
+            <a:t>2</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="4000">
             <a:solidFill>
@@ -13928,7 +13482,7 @@
             <a:rPr lang="en-US" sz="1200">
               <a:latin typeface="Berlin Sans FB" panose="020E0602020502020306" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Average Concentration</a:t>
+            <a:t>Average Optimsim</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="0">
@@ -14004,7 +13558,7 @@
             <a:rPr lang="en-US" sz="1200">
               <a:latin typeface="Berlin Sans FB" panose="020E0602020502020306" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Average Optimism</a:t>
+            <a:t>Average Concentration</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="0">
@@ -14086,7 +13640,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:t>4</a:t>
+            <a:t>5</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="4000">
             <a:solidFill>
@@ -14167,7 +13721,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:t>4</a:t>
+            <a:t>6</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="4000">
             <a:solidFill>
@@ -16853,10 +16407,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E5CF1904-7557-4CA1-9D08-B8591CE020AC}" name="average level of concentration" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="G38:G39" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{21E1D583-0ED3-4379-BF63-2280CB499671}" name="Concentration Level" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+  <location ref="B16:C18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="19">
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -16870,9 +16424,9 @@
     </pivotField>
     <pivotField showAll="0">
       <items count="4">
-        <item x="2"/>
+        <item h="1" x="2"/>
         <item x="1"/>
-        <item x="0"/>
+        <item h="1" x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -16897,13 +16451,224 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="9">
+        <item x="6"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="16"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="4" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ACB39330-5E08-44A0-A1CA-06F39D6DE222}" name="Sadness Level" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+  <location ref="F20:G21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="19">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="3"/>
         <item x="2"/>
+        <item x="1"/>
         <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
         <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item h="1" x="2"/>
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x v="2"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49D7CCB8-4B2C-4F7D-9640-4D011CC29AA7}" name="Average level of sexual activity" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F35:F36" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="19">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item h="1" x="2"/>
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
         <item x="3"/>
         <item t="default"/>
       </items>
@@ -16916,10 +16681,10 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Average of Concentration" fld="16" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of Sexual Activity" fld="15" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="96">
+    <format dxfId="41">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -16935,8 +16700,334 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3B23268-367F-44C7-93DB-AD41BE0D2B81}" name="PivotTable18" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2ABD9709-BA88-49DB-A34E-19FEDF1903BE}" name="Sexual Activity Level" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+  <location ref="J7:K8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="19">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item h="1" x="2"/>
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="10">
+        <item x="8"/>
+        <item x="7"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="15"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="3">
+    <chartFormat chart="3" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF3EE903-3031-431A-8802-56EF68DF5949}" name="Optimism Level" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="F7:G8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="19">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item h="1" x="2"/>
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="10">
+        <item x="8"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="17"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5B60E55B-B705-4BE3-A2E0-C51618093F88}" name="Expert Diagnosis" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="20">
+  <location ref="B7:C8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="19">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item h="1" x="2"/>
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="18"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x v="3"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="4" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3B23268-367F-44C7-93DB-AD41BE0D2B81}" name="PivotTable18" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B28:C39" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="19">
     <pivotField dataField="1" showAll="0"/>
@@ -17030,22 +17121,14 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{33438ED4-C5CE-45A7-93CD-A52DCDC8FA3E}" name="Exhaustion level" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
-  <location ref="F28:G32" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4CA7A061-250F-4EA6-9769-D6776205FD8B}" name="Number of Patients" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B2:B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="19">
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
@@ -17056,9 +17139,9 @@
     </pivotField>
     <pivotField showAll="0">
       <items count="4">
-        <item x="2"/>
+        <item h="1" x="2"/>
         <item x="1"/>
-        <item x="0"/>
+        <item h="1" x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -17087,9 +17170,95 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{33438ED4-C5CE-45A7-93CD-A52DCDC8FA3E}" name="Exhaustion level" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="F28:G29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="19">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="3"/>
         <item x="2"/>
         <item x="0"/>
         <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item h="1" x="2"/>
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
         <item x="3"/>
         <item t="default"/>
       </items>
@@ -17098,18 +17267,9 @@
   <rowFields count="1">
     <field x="3"/>
   </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
+  <rowItems count="1">
     <i>
       <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
     </i>
   </rowItems>
   <colItems count="1">
@@ -17159,23 +17319,23 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4F849281-9AB3-45E7-A339-C96EDF73C582}" name="Euphoric levels" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
-  <location ref="J20:K24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7A059DB6-E0C4-49B2-9545-AFB5043E0D09}" name="Sleep Disorder levels" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+  <location ref="J28:K30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="19">
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
         <item x="1"/>
+        <item x="3"/>
         <item x="0"/>
-        <item x="3"/>
         <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
         <item x="1"/>
@@ -17185,9 +17345,9 @@
     </pivotField>
     <pivotField showAll="0">
       <items count="4">
-        <item x="2"/>
+        <item h="1" x="2"/>
         <item x="1"/>
-        <item x="0"/>
+        <item h="1" x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -17216,9 +17376,280 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E5CF1904-7557-4CA1-9D08-B8591CE020AC}" name="average level of concentration" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="G38:G39" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="19">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item h="1" x="2"/>
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Concentration" fld="16" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="39">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F0311E1A-CB9A-47AD-8E54-841C2B6FE8D9}" name="average level of optimism" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F38:F39" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="19">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item h="1" x="2"/>
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Optimisim" fld="17" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="40">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4F849281-9AB3-45E7-A339-C96EDF73C582}" name="Euphoric levels" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+  <location ref="J20:K21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="19">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="3"/>
         <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
         <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item h="1" x="2"/>
         <item x="1"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
         <item x="3"/>
         <item t="default"/>
       </items>
@@ -17227,18 +17658,9 @@
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
+  <rowItems count="1">
     <i>
       <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
     </i>
   </rowItems>
   <colItems count="1">
@@ -17318,982 +17740,6 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2ABD9709-BA88-49DB-A34E-19FEDF1903BE}" name="Sexual Activity Level" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
-  <location ref="J7:K16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="19">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="10">
-        <item x="8"/>
-        <item x="7"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="15"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="3">
-    <chartFormat chart="3" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F0311E1A-CB9A-47AD-8E54-841C2B6FE8D9}" name="average level of optimism" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F38:F39" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="19">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Optimisim" fld="17" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="98">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49D7CCB8-4B2C-4F7D-9640-4D011CC29AA7}" name="Average level of sexual activity" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F35:F36" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="19">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Sexual Activity" fld="15" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="97">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5B60E55B-B705-4BE3-A2E0-C51618093F88}" name="Expert Diagnosis" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="20">
-  <location ref="B7:C11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="19">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="18"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="4" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4CA7A061-250F-4EA6-9769-D6776205FD8B}" name="Number of Patients" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B2:B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="19">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7A059DB6-E0C4-49B2-9545-AFB5043E0D09}" name="Sleep Disorder levels" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
-  <location ref="J28:K32" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="19">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ACB39330-5E08-44A0-A1CA-06F39D6DE222}" name="Sadness Level" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
-  <location ref="F20:G24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="19">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF3EE903-3031-431A-8802-56EF68DF5949}" name="Optimism Level" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="F7:G16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="19">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="10">
-        <item x="8"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="7"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="17"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{21E1D583-0ED3-4379-BF63-2280CB499671}" name="Concentration Level" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
-  <location ref="B16:C24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="19">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="9">
-        <item x="6"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="16"/>
-  </rowFields>
-  <rowItems count="8">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Patient Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="4" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Suicidal_thoughts" xr10:uid="{18FC8D42-4C69-4BB8-B1A9-A6A0B1191770}" sourceName="Suicidal thoughts">
   <pivotTables>
@@ -18313,9 +17759,9 @@
   <data>
     <tabular pivotCacheId="1778679977">
       <items count="3">
-        <i x="2" s="1"/>
+        <i x="2"/>
         <i x="1" s="1"/>
-        <i x="0" s="1"/>
+        <i x="0" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -18341,9 +17787,9 @@
   <data>
     <tabular pivotCacheId="1778679977">
       <items count="4">
-        <i x="2" s="1"/>
-        <i x="0" s="1"/>
-        <i x="1" s="1"/>
+        <i x="2"/>
+        <i x="0"/>
+        <i x="1"/>
         <i x="3" s="1"/>
       </items>
     </tabular>
@@ -18371,7 +17817,7 @@
     <tabular pivotCacheId="1778679977">
       <items count="2">
         <i x="1" s="1"/>
-        <i x="0" s="1"/>
+        <i x="0" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -18398,7 +17844,7 @@
     <tabular pivotCacheId="1778679977">
       <items count="2">
         <i x="1" s="1"/>
-        <i x="0" s="1"/>
+        <i x="0" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -33074,7 +32520,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
@@ -33089,8 +32535,8 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="5">
-        <v>120</v>
+      <c r="B3" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -33115,138 +32561,22 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="5">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2</v>
       </c>
       <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G8" s="6">
+        <v>2</v>
       </c>
       <c r="J8" s="2">
-        <v>1</v>
-      </c>
-      <c r="K8" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="5">
-        <v>31</v>
-      </c>
-      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="K8" s="6">
         <v>2</v>
-      </c>
-      <c r="G9" s="5">
-        <v>18</v>
-      </c>
-      <c r="J9" s="2">
-        <v>2</v>
-      </c>
-      <c r="K9" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="5">
-        <v>31</v>
-      </c>
-      <c r="F10" s="2">
-        <v>3</v>
-      </c>
-      <c r="G10" s="5">
-        <v>18</v>
-      </c>
-      <c r="J10" s="2">
-        <v>3</v>
-      </c>
-      <c r="K10" s="5">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="5">
-        <v>30</v>
-      </c>
-      <c r="F11" s="2">
-        <v>4</v>
-      </c>
-      <c r="G11" s="5">
-        <v>19</v>
-      </c>
-      <c r="J11" s="2">
-        <v>4</v>
-      </c>
-      <c r="K11" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F12" s="2">
-        <v>5</v>
-      </c>
-      <c r="G12" s="5">
-        <v>20</v>
-      </c>
-      <c r="J12" s="2">
-        <v>5</v>
-      </c>
-      <c r="K12" s="5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F13" s="2">
-        <v>6</v>
-      </c>
-      <c r="G13" s="5">
-        <v>21</v>
-      </c>
-      <c r="J13" s="2">
-        <v>6</v>
-      </c>
-      <c r="K13" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F14" s="2">
-        <v>7</v>
-      </c>
-      <c r="G14" s="5">
-        <v>8</v>
-      </c>
-      <c r="J14" s="2">
-        <v>7</v>
-      </c>
-      <c r="K14" s="5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F15" s="2">
-        <v>8</v>
-      </c>
-      <c r="G15" s="5">
-        <v>8</v>
-      </c>
-      <c r="J15" s="2">
-        <v>8</v>
-      </c>
-      <c r="K15" s="5">
-        <v>11</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
@@ -33256,50 +32586,24 @@
       <c r="C16" t="s">
         <v>281</v>
       </c>
-      <c r="F16" s="2">
-        <v>9</v>
-      </c>
-      <c r="G16" s="5">
-        <v>2</v>
-      </c>
-      <c r="J16" s="2">
-        <v>9</v>
-      </c>
-      <c r="K16" s="5">
-        <v>2</v>
-      </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6">
         <v>1</v>
-      </c>
-      <c r="C17" s="5">
-        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
-        <v>2</v>
-      </c>
-      <c r="C18" s="5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
-        <v>3</v>
-      </c>
-      <c r="C19" s="5">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
-        <v>4</v>
-      </c>
-      <c r="C20" s="5">
-        <v>33</v>
-      </c>
       <c r="F20" s="1" t="s">
         <v>279</v>
       </c>
@@ -33314,83 +32618,17 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
-        <v>5</v>
-      </c>
-      <c r="C21" s="5">
-        <v>21</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="5">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="G21" s="6">
+        <v>2</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" s="5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
-        <v>6</v>
-      </c>
-      <c r="C22" s="5">
-        <v>10</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="5">
-        <v>16</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="5">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
-        <v>7</v>
-      </c>
-      <c r="C23" s="5">
-        <v>14</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="5">
-        <v>42</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K23" s="5">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="2">
-        <v>8</v>
-      </c>
-      <c r="C24" s="5">
-        <v>4</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="5">
-        <v>42</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K24" s="5">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="K21" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -33417,87 +32655,57 @@
       <c r="B29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29">
         <v>70</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G29" s="5">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="G29" s="6">
+        <v>2</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K29" s="5">
         <v>21</v>
+      </c>
+      <c r="K29" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30">
         <v>6</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G30" s="5">
-        <v>18</v>
-      </c>
       <c r="J30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K30" s="5">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="K30" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="5">
-        <v>22</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G31" s="5">
-        <v>38</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K31" s="5">
-        <v>44</v>
+      <c r="C31">
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32">
         <v>29</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="5">
-        <v>34</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K32" s="5">
-        <v>34</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33">
         <v>13</v>
       </c>
     </row>
@@ -33505,7 +32713,7 @@
       <c r="B34" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34">
         <v>50</v>
       </c>
     </row>
@@ -33513,7 +32721,7 @@
       <c r="B35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35">
         <v>3</v>
       </c>
       <c r="F35" t="s">
@@ -33524,11 +32732,11 @@
       <c r="B36" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36">
         <v>24</v>
       </c>
-      <c r="F36" s="6">
-        <v>4.7416666666666663</v>
+      <c r="F36" s="5">
+        <v>5</v>
       </c>
       <c r="J36" s="2"/>
     </row>
@@ -33536,7 +32744,7 @@
       <c r="B37" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37">
         <v>16</v>
       </c>
       <c r="J37" s="2"/>
@@ -33545,7 +32753,7 @@
       <c r="B38" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38">
         <v>7</v>
       </c>
       <c r="F38" t="s">
@@ -33560,14 +32768,14 @@
       <c r="B39" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39">
         <v>120</v>
       </c>
-      <c r="F39" s="6">
-        <v>4.4666666666666668</v>
-      </c>
-      <c r="G39" s="6">
-        <v>4.25</v>
+      <c r="F39" s="5">
+        <v>5</v>
+      </c>
+      <c r="G39" s="5">
+        <v>5.5</v>
       </c>
       <c r="J39" s="2"/>
     </row>

</xml_diff>